<commit_message>
Done with Optimal Selection_ Split GOM vs SNE GPs. Only ranked OC within GOM regions
</commit_message>
<xml_diff>
--- a/TraitAnalyses201003/ReorderPedigree/Ped_in_Order_754-866_Individuals.xlsx
+++ b/TraitAnalyses201003/ReorderPedigree/Ped_in_Order_754-866_Individuals.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10600" yWindow="880" windowWidth="24480" windowHeight="14420" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="1940" yWindow="3120" windowWidth="24480" windowHeight="14420" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ped_in_Order_754_Individuals.cs" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6753" uniqueCount="940">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6754" uniqueCount="941">
   <si>
     <t>fndRow</t>
   </si>
@@ -2842,6 +2842,9 @@
   </si>
   <si>
     <t>&gt;   round(h2hMat,3)</t>
+  </si>
+  <si>
+    <t>included by 1-3 category</t>
   </si>
 </sst>
 </file>
@@ -60293,7 +60296,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -60342,6 +60345,9 @@
       </c>
       <c r="F5" s="6" t="s">
         <v>875</v>
+      </c>
+      <c r="G5" t="s">
+        <v>940</v>
       </c>
     </row>
     <row r="6" spans="1:10">

</xml_diff>